<commit_message>
Generic get files function
</commit_message>
<xml_diff>
--- a/docs/Examples/Example5_FI_density_to_depth/Fluid_Inclusion_Densities_Example1.xlsx
+++ b/docs/Examples/Example5_FI_density_to_depth/Fluid_Inclusion_Densities_Example1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Berkeley_NEW\DiadFit_outer\docs\Examples\Example5_FI_density_to_depth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B4C957-46C4-45DF-A88C-8D838F226E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1F6CCE-5567-43BF-B901-0FFF05F12E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15960" activeTab="1" xr2:uid="{70B86B56-DC75-4A25-AC0B-5B934F645505}"/>
   </bookViews>
@@ -873,7 +873,7 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -902,7 +902,7 @@
       </c>
       <c r="B2">
         <f ca="1">0.4+RAND()/10</f>
-        <v>0.46912897887061655</v>
+        <v>0.43688801914093245</v>
       </c>
       <c r="C2">
         <v>1048.8987375520094</v>
@@ -917,7 +917,7 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B39" ca="1" si="0">0.4+RAND()/10</f>
-        <v>0.4220261565439612</v>
+        <v>0.417795975145687</v>
       </c>
       <c r="C3">
         <v>1015.9247665279173</v>
@@ -932,7 +932,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49254799408148769</v>
+        <v>0.45904516284132113</v>
       </c>
       <c r="C4">
         <v>1041.5899157282199</v>
@@ -947,7 +947,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4800063616361101</v>
+        <v>0.49386495126176522</v>
       </c>
       <c r="C5">
         <v>1034.9351831687991</v>
@@ -962,7 +962,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.47351484701475133</v>
+        <v>0.48222653270397087</v>
       </c>
       <c r="C6">
         <v>1034.8201022056769</v>
@@ -977,7 +977,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4282238657271486</v>
+        <v>0.49044176269396944</v>
       </c>
       <c r="C7">
         <v>1030.5111317389017</v>
@@ -992,7 +992,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.40202663542849509</v>
+        <v>0.45378053293814441</v>
       </c>
       <c r="C8">
         <v>1037.9505598725484</v>
@@ -1007,7 +1007,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.47408614829122131</v>
+        <v>0.49193174573715692</v>
       </c>
       <c r="C9">
         <v>1015.7420222813428</v>
@@ -1022,7 +1022,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41550986958064329</v>
+        <v>0.44491759971525835</v>
       </c>
       <c r="C10">
         <v>1030.4199396576716</v>
@@ -1037,7 +1037,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.48170526538130465</v>
+        <v>0.49604250265848532</v>
       </c>
       <c r="C11">
         <v>1006.8181662935915</v>
@@ -1052,7 +1052,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45797464203238247</v>
+        <v>0.4999651493884455</v>
       </c>
       <c r="C12">
         <v>1026.760566084811</v>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49807089697592288</v>
+        <v>0.44783290899893585</v>
       </c>
       <c r="C13">
         <v>1014.5437767254358</v>
@@ -1082,7 +1082,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.42947685905461158</v>
+        <v>0.43432032079970101</v>
       </c>
       <c r="C14">
         <v>1014.5057860852271</v>
@@ -1097,7 +1097,7 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41314385779503116</v>
+        <v>0.48987657806937557</v>
       </c>
       <c r="C15">
         <v>1000.5222111680959</v>
@@ -1112,7 +1112,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.43828599105276489</v>
+        <v>0.44693263074506723</v>
       </c>
       <c r="C16">
         <v>1044.7840400802461</v>
@@ -1127,7 +1127,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45542031300032865</v>
+        <v>0.44759900013490939</v>
       </c>
       <c r="C17">
         <v>1038.1072564377114</v>
@@ -1142,7 +1142,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.43178557116634719</v>
+        <v>0.46691232772085506</v>
       </c>
       <c r="C18">
         <v>1003.0804891909572</v>
@@ -1157,7 +1157,7 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.46347239113762595</v>
+        <v>0.43681125381580832</v>
       </c>
       <c r="C19">
         <v>1036.8645225471666</v>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.43585470417741384</v>
+        <v>0.4706250057516238</v>
       </c>
       <c r="C20">
         <v>1007.3644263800718</v>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.47113542831211608</v>
+        <v>0.42626673678603577</v>
       </c>
       <c r="C21">
         <v>1007.0276924038382</v>
@@ -1202,7 +1202,7 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44028888242838859</v>
+        <v>0.43724240909877954</v>
       </c>
       <c r="C22">
         <v>1034.068338439359</v>
@@ -1217,7 +1217,7 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.47252347550868845</v>
+        <v>0.46653991580850246</v>
       </c>
       <c r="C23">
         <v>1025.5734052339465</v>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45758542355068305</v>
+        <v>0.48373019565959258</v>
       </c>
       <c r="C24">
         <v>1040.442842954038</v>
@@ -1247,7 +1247,7 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41305938344615972</v>
+        <v>0.419152127235076</v>
       </c>
       <c r="C25">
         <v>1021.6881602500816</v>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49882367062457172</v>
+        <v>0.41426181419918678</v>
       </c>
       <c r="C26">
         <v>1035.4802802553329</v>
@@ -1277,7 +1277,7 @@
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="0"/>
-        <v>0.42465483309373203</v>
+        <v>0.49377922887490933</v>
       </c>
       <c r="C27">
         <v>1011.6447589751147</v>
@@ -1292,7 +1292,7 @@
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.48256811582119497</v>
+        <v>0.42512696704990982</v>
       </c>
       <c r="C28">
         <v>1035.7310630756294</v>
@@ -1307,7 +1307,7 @@
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41331930910092146</v>
+        <v>0.46012436931893236</v>
       </c>
       <c r="C29">
         <v>1019.4447870413757</v>
@@ -1322,7 +1322,7 @@
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="0"/>
-        <v>0.42059889551255231</v>
+        <v>0.45442547835858743</v>
       </c>
       <c r="C30">
         <v>1034.3244254204421</v>
@@ -1337,7 +1337,7 @@
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="0"/>
-        <v>0.42381427258691862</v>
+        <v>0.44083547839660486</v>
       </c>
       <c r="C31">
         <v>1030.9788538090957</v>
@@ -1352,7 +1352,7 @@
       </c>
       <c r="B32">
         <f t="shared" ca="1" si="0"/>
-        <v>0.43632392675996989</v>
+        <v>0.4130949155539872</v>
       </c>
       <c r="C32">
         <v>1019.6265168236124</v>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="B33">
         <f t="shared" ca="1" si="0"/>
-        <v>0.40699686742218588</v>
+        <v>0.43305833984673581</v>
       </c>
       <c r="C33">
         <v>1030.2698548116346</v>
@@ -1382,7 +1382,7 @@
       </c>
       <c r="B34">
         <f t="shared" ca="1" si="0"/>
-        <v>0.42142208021007466</v>
+        <v>0.41417179991617487</v>
       </c>
       <c r="C34">
         <v>1031.4276080201123</v>
@@ -1397,7 +1397,7 @@
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4329163196877992</v>
+        <v>0.40041873149401319</v>
       </c>
       <c r="C35">
         <v>1039.10639320633</v>
@@ -1412,7 +1412,7 @@
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4419437695294014</v>
+        <v>0.40166102045343077</v>
       </c>
       <c r="C36">
         <v>1030.959574308064</v>
@@ -1427,7 +1427,7 @@
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41269508514659808</v>
+        <v>0.4270929298696502</v>
       </c>
       <c r="C37">
         <v>1040.1105447404047</v>
@@ -1442,7 +1442,7 @@
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="0"/>
-        <v>0.43657562561313534</v>
+        <v>0.49007133475856501</v>
       </c>
       <c r="C38">
         <v>1029.6585878004955</v>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="B39">
         <f t="shared" ca="1" si="0"/>
-        <v>0.48506390955171563</v>
+        <v>0.45812586127600197</v>
       </c>
       <c r="C39">
         <v>1000.948345450318</v>

</xml_diff>